<commit_message>
Displayed and exported execution time of the modules
</commit_message>
<xml_diff>
--- a/code/results/signal_reconstruction/counters_means.xlsx
+++ b/code/results/signal_reconstruction/counters_means.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>BR_INST_RETIRED</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>uops_dispatched:core</t>
+  </si>
+  <si>
+    <t>Path</t>
   </si>
 </sst>
 </file>
@@ -432,6 +435,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,58 +498,58 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>42688808.39393939</v>
+        <v>47813523.75862069</v>
       </c>
       <c r="C2">
-        <v>63701.15151515151</v>
+        <v>72031.93103448275</v>
       </c>
       <c r="D2">
-        <v>118303617.5757576</v>
+        <v>118338939.2758621</v>
       </c>
       <c r="E2">
-        <v>267082427.1212121</v>
+        <v>294408649.2413793</v>
       </c>
       <c r="F2">
-        <v>361640.8484848485</v>
+        <v>436425.3103448276</v>
       </c>
       <c r="G2">
-        <v>3766035.636363636</v>
+        <v>4222354.896551725</v>
       </c>
       <c r="H2">
-        <v>2869.606060606061</v>
+        <v>2622.241379310345</v>
       </c>
       <c r="I2">
-        <v>7912422.242424242</v>
+        <v>8578362.448275862</v>
       </c>
       <c r="J2">
-        <v>3847995.939393939</v>
+        <v>4154951.310344827</v>
       </c>
       <c r="K2">
-        <v>6746650.242424242</v>
+        <v>7329444.206896552</v>
       </c>
       <c r="L2">
-        <v>28685.24242424242</v>
+        <v>22236.03448275862</v>
       </c>
       <c r="M2">
-        <v>12437.9696969697</v>
+        <v>19231.27586206896</v>
       </c>
       <c r="N2">
-        <v>34576690.18181818</v>
+        <v>33804099.27586207</v>
       </c>
       <c r="O2">
-        <v>38055711.72727273</v>
+        <v>30668082.31034483</v>
       </c>
       <c r="P2">
-        <v>12.51515151515152</v>
+        <v>0.2758620689655172</v>
       </c>
       <c r="Q2">
-        <v>0.5454545454545454</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>15370996.93939394</v>
+        <v>11961100.31034483</v>
       </c>
       <c r="S2">
-        <v>353469369.4242424</v>
+        <v>337724498.9310345</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -551,58 +557,58 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>36120326.82051282</v>
+        <v>47493535.06666667</v>
       </c>
       <c r="C3">
-        <v>54282.5641025641</v>
+        <v>71735.56666666667</v>
       </c>
       <c r="D3">
-        <v>118716686.7948718</v>
+        <v>117723824.8666667</v>
       </c>
       <c r="E3">
-        <v>227010781.1025641</v>
+        <v>293220240.9666666</v>
       </c>
       <c r="F3">
-        <v>255892.5384615385</v>
+        <v>444926.6333333334</v>
       </c>
       <c r="G3">
-        <v>3089167.333333333</v>
+        <v>4214318.3</v>
       </c>
       <c r="H3">
-        <v>2259.410256410256</v>
+        <v>2619.533333333333</v>
       </c>
       <c r="I3">
-        <v>5978689.076923077</v>
+        <v>8607884</v>
       </c>
       <c r="J3">
-        <v>3386390.846153846</v>
+        <v>4182153.633333333</v>
       </c>
       <c r="K3">
-        <v>5963402.871794872</v>
+        <v>7348902.233333333</v>
       </c>
       <c r="L3">
-        <v>20560.20512820513</v>
+        <v>22606.16666666667</v>
       </c>
       <c r="M3">
-        <v>11015.94871794872</v>
+        <v>23952.73333333333</v>
       </c>
       <c r="N3">
-        <v>25890040.74358974</v>
+        <v>33724125.43333333</v>
       </c>
       <c r="O3">
-        <v>29873080.69230769</v>
+        <v>34501612.96666667</v>
       </c>
       <c r="P3">
-        <v>2.615384615384615</v>
+        <v>10.66666666666667</v>
       </c>
       <c r="Q3">
-        <v>0.4358974358974359</v>
+        <v>1.5</v>
       </c>
       <c r="R3">
-        <v>20742890.28205128</v>
+        <v>11973721.7</v>
       </c>
       <c r="S3">
-        <v>370402386.4871795</v>
+        <v>335698592.2666667</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -610,58 +616,58 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>6560648.747368421</v>
+        <v>11514819.9575</v>
       </c>
       <c r="C4">
-        <v>16819.69473684211</v>
+        <v>27154.0625</v>
       </c>
       <c r="D4">
-        <v>116664496.1894737</v>
+        <v>118075866.27</v>
       </c>
       <c r="E4">
-        <v>165321919.0736842</v>
+        <v>281895615.41</v>
       </c>
       <c r="F4">
-        <v>145540.9368421053</v>
+        <v>107768.01</v>
       </c>
       <c r="G4">
-        <v>798038.8421052631</v>
+        <v>1168080.97</v>
       </c>
       <c r="H4">
-        <v>721130.7368421053</v>
+        <v>1221751.68</v>
       </c>
       <c r="I4">
-        <v>3733126.884210526</v>
+        <v>5501275.015</v>
       </c>
       <c r="J4">
-        <v>2792863.484210526</v>
+        <v>4063163.9675</v>
       </c>
       <c r="K4">
-        <v>3452840.042105263</v>
+        <v>4957122.65</v>
       </c>
       <c r="L4">
-        <v>96369.96842105263</v>
+        <v>137673.89</v>
       </c>
       <c r="M4">
-        <v>12840.28421052632</v>
+        <v>17605.8</v>
       </c>
       <c r="N4">
-        <v>8985162.842105264</v>
+        <v>14153410.1375</v>
       </c>
       <c r="O4">
-        <v>10048406.38947368</v>
+        <v>14223883.47</v>
       </c>
       <c r="P4">
-        <v>4.631578947368421</v>
+        <v>0.9</v>
       </c>
       <c r="Q4">
-        <v>12.52631578947368</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>29760886.54736842</v>
+        <v>33404318.135</v>
       </c>
       <c r="S4">
-        <v>355697497.1578947</v>
+        <v>349952572.0675</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -669,58 +675,58 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>6449087.610526316</v>
+        <v>11501709.805</v>
       </c>
       <c r="C5">
-        <v>16173.61052631579</v>
+        <v>27078.52</v>
       </c>
       <c r="D5">
-        <v>118990730.2315789</v>
+        <v>118091567.1275</v>
       </c>
       <c r="E5">
-        <v>163322122.1052631</v>
+        <v>281205886.185</v>
       </c>
       <c r="F5">
-        <v>178214.9578947368</v>
+        <v>105813.4075</v>
       </c>
       <c r="G5">
-        <v>858519.2526315789</v>
+        <v>1157808.07</v>
       </c>
       <c r="H5">
-        <v>657868.652631579</v>
+        <v>1225466.2075</v>
       </c>
       <c r="I5">
-        <v>3382885.136842105</v>
+        <v>5487156.13</v>
       </c>
       <c r="J5">
-        <v>2618236.431578947</v>
+        <v>4059552.8875</v>
       </c>
       <c r="K5">
-        <v>3389214.010526316</v>
+        <v>4948339.98</v>
       </c>
       <c r="L5">
-        <v>88528.57894736843</v>
+        <v>137559.22</v>
       </c>
       <c r="M5">
-        <v>12095.50526315789</v>
+        <v>17010.8</v>
       </c>
       <c r="N5">
-        <v>8483048.768421052</v>
+        <v>14116170.92</v>
       </c>
       <c r="O5">
-        <v>9193398.168421052</v>
+        <v>14186769.655</v>
       </c>
       <c r="P5">
-        <v>2.347368421052632</v>
+        <v>0.295</v>
       </c>
       <c r="Q5">
-        <v>12.33684210526316</v>
+        <v>0.135</v>
       </c>
       <c r="R5">
-        <v>31258316.75789474</v>
+        <v>33528742.66</v>
       </c>
       <c r="S5">
-        <v>355772289.4210526</v>
+        <v>349205785.8375</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -728,58 +734,58 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>9267750.263157895</v>
+        <v>9289535.1075</v>
       </c>
       <c r="C6">
-        <v>7280.2</v>
+        <v>8719.077499999999</v>
       </c>
       <c r="D6">
-        <v>124859754.4421053</v>
+        <v>118112314.0925</v>
       </c>
       <c r="E6">
-        <v>250952907.7263158</v>
+        <v>245403858.865</v>
       </c>
       <c r="F6">
-        <v>78439.68421052632</v>
+        <v>77893.16499999999</v>
       </c>
       <c r="G6">
-        <v>172101.7894736842</v>
+        <v>161669.27</v>
       </c>
       <c r="H6">
-        <v>1461030.2</v>
+        <v>1455328.7875</v>
       </c>
       <c r="I6">
-        <v>7568462.505263158</v>
+        <v>7620081.25</v>
       </c>
       <c r="J6">
-        <v>3244124.442105263</v>
+        <v>3273565.3925</v>
       </c>
       <c r="K6">
-        <v>3356286.347368421</v>
+        <v>3388278.2625</v>
       </c>
       <c r="L6">
-        <v>33799.0947368421</v>
+        <v>19756.685</v>
       </c>
       <c r="M6">
-        <v>12303.95789473684</v>
+        <v>15661.6825</v>
       </c>
       <c r="N6">
-        <v>39969814.36842106</v>
+        <v>40746702.71</v>
       </c>
       <c r="O6">
-        <v>45659767.11578947</v>
+        <v>40906648.835</v>
       </c>
       <c r="P6">
-        <v>0.4947368421052631</v>
+        <v>1.0575</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>0.99</v>
       </c>
       <c r="R6">
-        <v>28598614.91578947</v>
+        <v>29606698.76</v>
       </c>
       <c r="S6">
-        <v>333996583.968421</v>
+        <v>327551465.3075</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -787,58 +793,58 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>7916593.789473685</v>
+        <v>9268455.074999999</v>
       </c>
       <c r="C7">
-        <v>7392.18947368421</v>
+        <v>8580.01</v>
       </c>
       <c r="D7">
-        <v>118737160.3894737</v>
+        <v>118096212.9075</v>
       </c>
       <c r="E7">
-        <v>210420907.6</v>
+        <v>244869860.6025</v>
       </c>
       <c r="F7">
-        <v>58558.75789473685</v>
+        <v>74063.1075</v>
       </c>
       <c r="G7">
-        <v>221278.9894736842</v>
+        <v>162231.9875</v>
       </c>
       <c r="H7">
-        <v>1245751.252631579</v>
+        <v>1452515.79</v>
       </c>
       <c r="I7">
-        <v>6878569.810526316</v>
+        <v>7614514.4875</v>
       </c>
       <c r="J7">
-        <v>2802379.263157895</v>
+        <v>3280486.7525</v>
       </c>
       <c r="K7">
-        <v>2989155.505263158</v>
+        <v>3392888.24</v>
       </c>
       <c r="L7">
-        <v>77061.65263157895</v>
+        <v>22152.4125</v>
       </c>
       <c r="M7">
-        <v>17902.01052631579</v>
+        <v>17532.7225</v>
       </c>
       <c r="N7">
-        <v>36417420.01052631</v>
+        <v>40658370.2425</v>
       </c>
       <c r="O7">
-        <v>37118696.12631579</v>
+        <v>40816750.4825</v>
       </c>
       <c r="P7">
-        <v>0.5684210526315789</v>
+        <v>0.045</v>
       </c>
       <c r="Q7">
-        <v>5.494736842105263</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>26518820.11578947</v>
+        <v>29934915.2975</v>
       </c>
       <c r="S7">
-        <v>342028450.1263158</v>
+        <v>326643413.49</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -846,58 +852,58 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>6943599.231578947</v>
+        <v>9255591.942500001</v>
       </c>
       <c r="C8">
-        <v>8487.673684210526</v>
+        <v>9295.385</v>
       </c>
       <c r="D8">
-        <v>122956091.5157895</v>
+        <v>118129576.265</v>
       </c>
       <c r="E8">
-        <v>180974562.3052632</v>
+        <v>246773077.5675</v>
       </c>
       <c r="F8">
-        <v>94730.2947368421</v>
+        <v>131055.6725</v>
       </c>
       <c r="G8">
-        <v>984368.6210526315</v>
+        <v>796583.84</v>
       </c>
       <c r="H8">
-        <v>2836.673684210527</v>
+        <v>2616.44</v>
       </c>
       <c r="I8">
-        <v>6908239.578947368</v>
+        <v>9584770.9375</v>
       </c>
       <c r="J8">
-        <v>3089032.715789474</v>
+        <v>4717772.7975</v>
       </c>
       <c r="K8">
-        <v>3876900.968421053</v>
+        <v>5386608.59</v>
       </c>
       <c r="L8">
-        <v>190315.3157894737</v>
+        <v>101570.43</v>
       </c>
       <c r="M8">
-        <v>18465.4</v>
+        <v>21402.0475</v>
       </c>
       <c r="N8">
-        <v>29262929.72631579</v>
+        <v>40580067.88</v>
       </c>
       <c r="O8">
-        <v>34395956.76842105</v>
+        <v>40746575.2175</v>
       </c>
       <c r="P8">
-        <v>12.16842105263158</v>
+        <v>2.6325</v>
       </c>
       <c r="Q8">
-        <v>0.8105263157894737</v>
+        <v>2.0925</v>
       </c>
       <c r="R8">
-        <v>26401791.81052632</v>
+        <v>27490339.06</v>
       </c>
       <c r="S8">
-        <v>350782380.8631579</v>
+        <v>332489077.115</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -905,58 +911,58 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>8729587.378947368</v>
+        <v>9253786.68</v>
       </c>
       <c r="C9">
-        <v>7614.978947368421</v>
+        <v>8401.922500000001</v>
       </c>
       <c r="D9">
-        <v>121029302.8736842</v>
+        <v>118190482.91</v>
       </c>
       <c r="E9">
-        <v>228402096.7368421</v>
+        <v>246782029.1525</v>
       </c>
       <c r="F9">
-        <v>117845.6736842105</v>
+        <v>134816.22</v>
       </c>
       <c r="G9">
-        <v>1011296.505263158</v>
+        <v>846384.3175</v>
       </c>
       <c r="H9">
-        <v>2865.431578947369</v>
+        <v>2627.36</v>
       </c>
       <c r="I9">
-        <v>8695947.368421054</v>
+        <v>9591199.244999999</v>
       </c>
       <c r="J9">
-        <v>4125736.47368421</v>
+        <v>4684875.88</v>
       </c>
       <c r="K9">
-        <v>4997532.326315789</v>
+        <v>5391748.6875</v>
       </c>
       <c r="L9">
-        <v>192391.3157894737</v>
+        <v>112444.845</v>
       </c>
       <c r="M9">
-        <v>18469.12631578948</v>
+        <v>19248.4</v>
       </c>
       <c r="N9">
-        <v>36651162.85263158</v>
+        <v>40561000.975</v>
       </c>
       <c r="O9">
-        <v>37253816.90526316</v>
+        <v>40728573.4125</v>
       </c>
       <c r="P9">
-        <v>0.1684210526315789</v>
+        <v>0.1575</v>
       </c>
       <c r="Q9">
-        <v>5.926315789473684</v>
+        <v>0</v>
       </c>
       <c r="R9">
-        <v>28644267.8</v>
+        <v>27744699.135</v>
       </c>
       <c r="S9">
-        <v>335573218.0421053</v>
+        <v>331656562.5425</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -964,58 +970,58 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>5631021.242105263</v>
+        <v>9442724.9925</v>
       </c>
       <c r="C10">
-        <v>6482.052631578948</v>
+        <v>9009.5075</v>
       </c>
       <c r="D10">
-        <v>116051640.1578947</v>
+        <v>118040785.8025</v>
       </c>
       <c r="E10">
-        <v>142944938.0421053</v>
+        <v>250033220.325</v>
       </c>
       <c r="F10">
-        <v>73652.78947368421</v>
+        <v>144821.28</v>
       </c>
       <c r="G10">
-        <v>1012368.252631579</v>
+        <v>723013.3075</v>
       </c>
       <c r="H10">
-        <v>676077.7263157895</v>
+        <v>1240467.1775</v>
       </c>
       <c r="I10">
-        <v>5161789.621052631</v>
+        <v>9662250.0875</v>
       </c>
       <c r="J10">
-        <v>2249037.852631579</v>
+        <v>4719576.2475</v>
       </c>
       <c r="K10">
-        <v>3067472.663157895</v>
+        <v>5368809.7</v>
       </c>
       <c r="L10">
-        <v>209624.9157894737</v>
+        <v>49584.325</v>
       </c>
       <c r="M10">
-        <v>16018.18947368421</v>
+        <v>21576.6475</v>
       </c>
       <c r="N10">
-        <v>24163215.21052632</v>
+        <v>41446264.325</v>
       </c>
       <c r="O10">
-        <v>25040309.42105263</v>
+        <v>41625250.85</v>
       </c>
       <c r="P10">
-        <v>7.242105263157895</v>
+        <v>0.2025</v>
       </c>
       <c r="Q10">
-        <v>0.6105263157894737</v>
+        <v>0</v>
       </c>
       <c r="R10">
-        <v>29579896.52631579</v>
+        <v>26272073.3775</v>
       </c>
       <c r="S10">
-        <v>377493866.968421</v>
+        <v>335923722.1025</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -1023,58 +1029,58 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>6026201.242105263</v>
+        <v>9479049.8225</v>
       </c>
       <c r="C11">
-        <v>7107.821052631579</v>
+        <v>9165.93</v>
       </c>
       <c r="D11">
-        <v>116921638.5578947</v>
+        <v>118049777.875</v>
       </c>
       <c r="E11">
-        <v>156335973.2631579</v>
+        <v>250927424.6575</v>
       </c>
       <c r="F11">
-        <v>82671.98947368421</v>
+        <v>155141.86</v>
       </c>
       <c r="G11">
-        <v>1004958.073684211</v>
+        <v>690535.6</v>
       </c>
       <c r="H11">
-        <v>773359.6105263158</v>
+        <v>1245050.8425</v>
       </c>
       <c r="I11">
-        <v>6083532.978947368</v>
+        <v>9692556.76</v>
       </c>
       <c r="J11">
-        <v>2589140.252631579</v>
+        <v>4753358.63</v>
       </c>
       <c r="K11">
-        <v>3311007.336842105</v>
+        <v>5385137.8175</v>
       </c>
       <c r="L11">
-        <v>173353</v>
+        <v>35673.05</v>
       </c>
       <c r="M11">
-        <v>19341.81052631579</v>
+        <v>22671.6525</v>
       </c>
       <c r="N11">
-        <v>26711738.4631579</v>
+        <v>41581913.9475</v>
       </c>
       <c r="O11">
-        <v>27163020.6631579</v>
+        <v>41764703.7225</v>
       </c>
       <c r="P11">
-        <v>8.863157894736842</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="Q11">
-        <v>11.36842105263158</v>
+        <v>0.54</v>
       </c>
       <c r="R11">
-        <v>27377965.11578947</v>
+        <v>25954802.6475</v>
       </c>
       <c r="S11">
-        <v>341610284.5368421</v>
+        <v>337053740.0425</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -1082,58 +1088,58 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>8983716</v>
+        <v>10700982.33333333</v>
       </c>
       <c r="C12">
-        <v>36673.66666666666</v>
+        <v>38930.33333333334</v>
       </c>
       <c r="D12">
-        <v>114127887.3333333</v>
+        <v>114595491.6666667</v>
       </c>
       <c r="E12">
-        <v>242042807</v>
+        <v>247558418</v>
       </c>
       <c r="F12">
-        <v>581659</v>
+        <v>656307.3333333334</v>
       </c>
       <c r="G12">
-        <v>1366556.333333333</v>
+        <v>1304196.666666667</v>
       </c>
       <c r="H12">
-        <v>1207613.333333333</v>
+        <v>1256845.666666667</v>
       </c>
       <c r="I12">
-        <v>4809676.666666667</v>
+        <v>4708554</v>
       </c>
       <c r="J12">
-        <v>3041934.666666667</v>
+        <v>3315340.333333333</v>
       </c>
       <c r="K12">
-        <v>3544596</v>
+        <v>3862461.333333333</v>
       </c>
       <c r="L12">
-        <v>621424</v>
+        <v>527582.3333333334</v>
       </c>
       <c r="M12">
-        <v>23958.33333333333</v>
+        <v>23919.33333333333</v>
       </c>
       <c r="N12">
-        <v>13008871</v>
+        <v>13172007.66666667</v>
       </c>
       <c r="O12">
-        <v>15149604</v>
+        <v>15775042.33333333</v>
       </c>
       <c r="P12">
-        <v>5.333333333333333</v>
+        <v>3</v>
       </c>
       <c r="Q12">
-        <v>409</v>
+        <v>0</v>
       </c>
       <c r="R12">
-        <v>36912244.66666666</v>
+        <v>36439764.33333334</v>
       </c>
       <c r="S12">
-        <v>346377164.6666667</v>
+        <v>340144186</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1141,58 +1147,58 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>7787798.25</v>
+        <v>10590200.33333333</v>
       </c>
       <c r="C13">
-        <v>30312.5</v>
+        <v>40406</v>
       </c>
       <c r="D13">
-        <v>116332582.75</v>
+        <v>115762663.6666667</v>
       </c>
       <c r="E13">
-        <v>218936069.75</v>
+        <v>247686679.6666667</v>
       </c>
       <c r="F13">
-        <v>440939.25</v>
+        <v>686723.6666666666</v>
       </c>
       <c r="G13">
-        <v>1251183</v>
+        <v>1296446.333333333</v>
       </c>
       <c r="H13">
-        <v>1010452</v>
+        <v>1096938.666666667</v>
       </c>
       <c r="I13">
-        <v>5075085</v>
+        <v>4711709.666666667</v>
       </c>
       <c r="J13">
-        <v>3525346.75</v>
+        <v>3292987.333333333</v>
       </c>
       <c r="K13">
-        <v>4005591.75</v>
+        <v>3819518.333333333</v>
       </c>
       <c r="L13">
-        <v>523978.5</v>
+        <v>528560.3333333334</v>
       </c>
       <c r="M13">
-        <v>16922.25</v>
+        <v>28836.66666666667</v>
       </c>
       <c r="N13">
-        <v>10659321.25</v>
+        <v>13184698</v>
       </c>
       <c r="O13">
-        <v>12540977.75</v>
+        <v>15576739.33333333</v>
       </c>
       <c r="P13">
-        <v>2.25</v>
+        <v>19.33333333333333</v>
       </c>
       <c r="Q13">
-        <v>386.25</v>
+        <v>0</v>
       </c>
       <c r="R13">
-        <v>34878262.5</v>
+        <v>35966287</v>
       </c>
       <c r="S13">
-        <v>354769900.5</v>
+        <v>340186211</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -1200,58 +1206,58 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>3433201.936842105</v>
+        <v>6098843.28</v>
       </c>
       <c r="C14">
-        <v>5863.81052631579</v>
+        <v>9768.6675</v>
       </c>
       <c r="D14">
-        <v>113260910.2315789</v>
+        <v>118166435.175</v>
       </c>
       <c r="E14">
-        <v>153605234.6526316</v>
+        <v>279513961.385</v>
       </c>
       <c r="F14">
-        <v>10141.43157894737</v>
+        <v>8281.5525</v>
       </c>
       <c r="G14">
-        <v>283594.5789473684</v>
+        <v>84148.34</v>
       </c>
       <c r="H14">
-        <v>2273039.368421053</v>
+        <v>3896057.5125</v>
       </c>
       <c r="I14">
-        <v>3393542.747368421</v>
+        <v>5707761.5375</v>
       </c>
       <c r="J14">
-        <v>1824550.431578947</v>
+        <v>3127792.3275</v>
       </c>
       <c r="K14">
-        <v>2020186.536842105</v>
+        <v>3170413.5475</v>
       </c>
       <c r="L14">
-        <v>120526.0526315789</v>
+        <v>13591.685</v>
       </c>
       <c r="M14">
-        <v>21309.24210526316</v>
+        <v>25752.0175</v>
       </c>
       <c r="N14">
-        <v>29857565.95789474</v>
+        <v>46669831.535</v>
       </c>
       <c r="O14">
-        <v>31193580.34736842</v>
+        <v>46862051.735</v>
       </c>
       <c r="P14">
-        <v>8.821052631578947</v>
+        <v>5.49</v>
       </c>
       <c r="Q14">
-        <v>0.5263157894736842</v>
+        <v>1.35</v>
       </c>
       <c r="R14">
-        <v>21875955.44210526</v>
+        <v>27772195.885</v>
       </c>
       <c r="S14">
-        <v>369107418.0631579</v>
+        <v>362416719.2125</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -1259,58 +1265,58 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>3322342.92631579</v>
+        <v>5857024.45</v>
       </c>
       <c r="C15">
-        <v>4854.789473684211</v>
+        <v>7069.4025</v>
       </c>
       <c r="D15">
-        <v>114605887.3368421</v>
+        <v>118066228.4025</v>
       </c>
       <c r="E15">
-        <v>149973333.6526316</v>
+        <v>270847741.4825</v>
       </c>
       <c r="F15">
-        <v>46962.13684210526</v>
+        <v>66112.9575</v>
       </c>
       <c r="G15">
-        <v>956140.8421052631</v>
+        <v>528329.99</v>
       </c>
       <c r="H15">
-        <v>1578505.568421053</v>
+        <v>2801935.37</v>
       </c>
       <c r="I15">
-        <v>3578030.378947368</v>
+        <v>6860279.4925</v>
       </c>
       <c r="J15">
-        <v>1883076.231578947</v>
+        <v>3996851.9925</v>
       </c>
       <c r="K15">
-        <v>2682254.642105263</v>
+        <v>4423687.635</v>
       </c>
       <c r="L15">
-        <v>230177.2210526316</v>
+        <v>67757.4525</v>
       </c>
       <c r="M15">
-        <v>22712.8</v>
+        <v>31532.6325</v>
       </c>
       <c r="N15">
-        <v>26512649.38947368</v>
+        <v>44832674.9425</v>
       </c>
       <c r="O15">
-        <v>26689581.34736842</v>
+        <v>45026490.51</v>
       </c>
       <c r="P15">
-        <v>15.89473684210526</v>
+        <v>2.295</v>
       </c>
       <c r="Q15">
-        <v>12.83157894736842</v>
+        <v>2.025</v>
       </c>
       <c r="R15">
-        <v>27723054.37894737</v>
+        <v>32101155.9975</v>
       </c>
       <c r="S15">
-        <v>357771587.6210526</v>
+        <v>351157872.6825</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -1318,58 +1324,58 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>4806759.389473684</v>
+        <v>5881679.7625</v>
       </c>
       <c r="C16">
-        <v>6534.536842105264</v>
+        <v>6086.735</v>
       </c>
       <c r="D16">
-        <v>121113435.5473684</v>
+        <v>118033938.22</v>
       </c>
       <c r="E16">
-        <v>221502266.8842105</v>
+        <v>271518644.5075</v>
       </c>
       <c r="F16">
-        <v>76893.42105263157</v>
+        <v>85310.375</v>
       </c>
       <c r="G16">
-        <v>725794.347368421</v>
+        <v>621156.785</v>
       </c>
       <c r="H16">
-        <v>2995691.336842105</v>
+        <v>3552030.825</v>
       </c>
       <c r="I16">
-        <v>5871546.694736842</v>
+        <v>6845907.9875</v>
       </c>
       <c r="J16">
-        <v>2978956.978947368</v>
+        <v>3870409.56</v>
       </c>
       <c r="K16">
-        <v>3682470.715789474</v>
+        <v>4390296.9375</v>
       </c>
       <c r="L16">
-        <v>121748.3157894737</v>
+        <v>72542.99249999999</v>
       </c>
       <c r="M16">
-        <v>21939.54736842105</v>
+        <v>26732.955</v>
       </c>
       <c r="N16">
-        <v>36901777.04210526</v>
+        <v>45558663.3275</v>
       </c>
       <c r="O16">
-        <v>40160387.76842105</v>
+        <v>45750105.255</v>
       </c>
       <c r="P16">
-        <v>1.210526315789474</v>
+        <v>0.7875</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="R16">
-        <v>29392946.45263158</v>
+        <v>31472965.7725</v>
       </c>
       <c r="S16">
-        <v>354510912.6105263</v>
+        <v>352558393.7025</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -1377,58 +1383,58 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>8476624.221052632</v>
+        <v>9270318.3125</v>
       </c>
       <c r="C17">
-        <v>7033.421052631579</v>
+        <v>6418.725</v>
       </c>
       <c r="D17">
-        <v>117802018.4210526</v>
+        <v>118070018.7425</v>
       </c>
       <c r="E17">
-        <v>223744088.2947368</v>
+        <v>245406593.805</v>
       </c>
       <c r="F17">
-        <v>64454.76842105263</v>
+        <v>70459.9425</v>
       </c>
       <c r="G17">
-        <v>177241.3684210526</v>
+        <v>156227.8475</v>
       </c>
       <c r="H17">
-        <v>1284911.473684211</v>
+        <v>1388652.02</v>
       </c>
       <c r="I17">
-        <v>7006480.621052631</v>
+        <v>7650164.45</v>
       </c>
       <c r="J17">
-        <v>3068133.557894737</v>
+        <v>3317111.5175</v>
       </c>
       <c r="K17">
-        <v>3309892.936842105</v>
+        <v>3421738.4825</v>
       </c>
       <c r="L17">
-        <v>42432.6</v>
+        <v>25456.875</v>
       </c>
       <c r="M17">
-        <v>16323.52631578947</v>
+        <v>19241.995</v>
       </c>
       <c r="N17">
-        <v>38775120.88421053</v>
+        <v>40725359.025</v>
       </c>
       <c r="O17">
-        <v>43633386.04210526</v>
+        <v>40894358.5275</v>
       </c>
       <c r="P17">
-        <v>0.09473684210526316</v>
+        <v>1.53</v>
       </c>
       <c r="Q17">
-        <v>12.46315789473684</v>
+        <v>1.0575</v>
       </c>
       <c r="R17">
-        <v>22857886.76842105</v>
+        <v>24164039.125</v>
       </c>
       <c r="S17">
-        <v>340264321.7157895</v>
+        <v>329900438.3825</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -1436,58 +1442,58 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>8307300.294736842</v>
+        <v>9351414.6975</v>
       </c>
       <c r="C18">
-        <v>7851</v>
+        <v>8796.004999999999</v>
       </c>
       <c r="D18">
-        <v>121524834.6</v>
+        <v>118075682.8225</v>
       </c>
       <c r="E18">
-        <v>222331726.8631579</v>
+        <v>249965705.885</v>
       </c>
       <c r="F18">
-        <v>117282.6842105263</v>
+        <v>148746.935</v>
       </c>
       <c r="G18">
-        <v>952854.5894736842</v>
+        <v>665483.9175</v>
       </c>
       <c r="H18">
-        <v>45221.61052631579</v>
+        <v>50472.305</v>
       </c>
       <c r="I18">
-        <v>8391085.810526315</v>
+        <v>9718550.797499999</v>
       </c>
       <c r="J18">
-        <v>3926038.673684211</v>
+        <v>4881607.98</v>
       </c>
       <c r="K18">
-        <v>4588036.052631579</v>
+        <v>5473957.665</v>
       </c>
       <c r="L18">
-        <v>150328.0105263158</v>
+        <v>46539.9925</v>
       </c>
       <c r="M18">
-        <v>20485.2947368421</v>
+        <v>25396.99</v>
       </c>
       <c r="N18">
-        <v>35855297.25263158</v>
+        <v>41123677.3875</v>
       </c>
       <c r="O18">
-        <v>41575237.67368421</v>
+        <v>41292794.1825</v>
       </c>
       <c r="P18">
-        <v>4.294736842105263</v>
+        <v>1.035</v>
       </c>
       <c r="Q18">
-        <v>1.052631578947368</v>
+        <v>1.215</v>
       </c>
       <c r="R18">
-        <v>25738819.70526316</v>
+        <v>24540059.435</v>
       </c>
       <c r="S18">
-        <v>332975022.3052632</v>
+        <v>338517311.7925</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -1495,58 +1501,58 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>5354082.947368421</v>
+        <v>9193402.564999999</v>
       </c>
       <c r="C19">
-        <v>6185.463157894736</v>
+        <v>9000.094999999999</v>
       </c>
       <c r="D19">
-        <v>115348828.0105263</v>
+        <v>117977392.25</v>
       </c>
       <c r="E19">
-        <v>140400668.9894737</v>
+        <v>244003873.7375</v>
       </c>
       <c r="F19">
-        <v>68295.87368421053</v>
+        <v>124642.8375</v>
       </c>
       <c r="G19">
-        <v>1168892.010526316</v>
+        <v>994976.4175</v>
       </c>
       <c r="H19">
-        <v>734469.0315789473</v>
+        <v>1288943.005</v>
       </c>
       <c r="I19">
-        <v>5495754.810526316</v>
+        <v>9460719.145</v>
       </c>
       <c r="J19">
-        <v>2247809.778947368</v>
+        <v>4467824.8025</v>
       </c>
       <c r="K19">
-        <v>3323018.852631579</v>
+        <v>5270824.54</v>
       </c>
       <c r="L19">
-        <v>250316.0947368421</v>
+        <v>160787.7675</v>
       </c>
       <c r="M19">
-        <v>18617.92631578947</v>
+        <v>24656.62</v>
       </c>
       <c r="N19">
-        <v>23297386.8</v>
+        <v>40428242.2525</v>
       </c>
       <c r="O19">
-        <v>24471837.12631579</v>
+        <v>37290034.97</v>
       </c>
       <c r="P19">
-        <v>2.610526315789474</v>
+        <v>0.0475</v>
       </c>
       <c r="Q19">
-        <v>1.08421052631579</v>
+        <v>0.0225</v>
       </c>
       <c r="R19">
-        <v>27648888.06315789</v>
+        <v>27547939.03</v>
       </c>
       <c r="S19">
-        <v>336304854.5789474</v>
+        <v>330596671.81</v>
       </c>
     </row>
     <row r="20" spans="1:19">
@@ -1554,58 +1560,58 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>9250548.357894737</v>
+        <v>9305817.6625</v>
       </c>
       <c r="C20">
-        <v>7509.8</v>
+        <v>8445.785</v>
       </c>
       <c r="D20">
-        <v>124931013.4</v>
+        <v>118148119.3325</v>
       </c>
       <c r="E20">
-        <v>244162977.9052632</v>
+        <v>244194923.97</v>
       </c>
       <c r="F20">
-        <v>70820.88421052632</v>
+        <v>75498.63250000001</v>
       </c>
       <c r="G20">
-        <v>190938.6947368421</v>
+        <v>146051.5025</v>
       </c>
       <c r="H20">
-        <v>1240866.473684211</v>
+        <v>1320835.68</v>
       </c>
       <c r="I20">
-        <v>7336352.347368421</v>
+        <v>7633135.4875</v>
       </c>
       <c r="J20">
-        <v>3132889.031578947</v>
+        <v>3275643.2975</v>
       </c>
       <c r="K20">
-        <v>3233174.831578947</v>
+        <v>3380720.8725</v>
       </c>
       <c r="L20">
-        <v>57834.8</v>
+        <v>17313.7875</v>
       </c>
       <c r="M20">
-        <v>13922.6</v>
+        <v>17232.655</v>
       </c>
       <c r="N20">
-        <v>39263603.93684211</v>
+        <v>40779356.5775</v>
       </c>
       <c r="O20">
-        <v>34005366.81052632</v>
+        <v>40967768.57</v>
       </c>
       <c r="P20">
-        <v>0.6210526315789474</v>
+        <v>2.0475</v>
       </c>
       <c r="Q20">
-        <v>16.95789473684211</v>
+        <v>1.215</v>
       </c>
       <c r="R20">
-        <v>27403724.55789474</v>
+        <v>28413763.59</v>
       </c>
       <c r="S20">
-        <v>339617975.968421</v>
+        <v>328371085.0525</v>
       </c>
     </row>
     <row r="21" spans="1:19">
@@ -1613,58 +1619,58 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>5529337.389473684</v>
+        <v>9358330.055</v>
       </c>
       <c r="C21">
-        <v>6099.18947368421</v>
+        <v>9029.4725</v>
       </c>
       <c r="D21">
-        <v>114458416.0315789</v>
+        <v>118106334.5425</v>
       </c>
       <c r="E21">
-        <v>140892546.7894737</v>
+        <v>247847905.8025</v>
       </c>
       <c r="F21">
-        <v>69568.12631578947</v>
+        <v>140825.2375</v>
       </c>
       <c r="G21">
-        <v>1448919.326315789</v>
+        <v>695299.0825</v>
       </c>
       <c r="H21">
-        <v>2890.642105263158</v>
+        <v>2629.4275</v>
       </c>
       <c r="I21">
-        <v>5659698.368421053</v>
+        <v>9661229.25</v>
       </c>
       <c r="J21">
-        <v>2267433.021052632</v>
+        <v>4783165.845</v>
       </c>
       <c r="K21">
-        <v>3372532.715789474</v>
+        <v>5392798.4325</v>
       </c>
       <c r="L21">
-        <v>405906.1789473684</v>
+        <v>60131.1175</v>
       </c>
       <c r="M21">
-        <v>18196.22105263158</v>
+        <v>22653.3725</v>
       </c>
       <c r="N21">
-        <v>23749747.43157895</v>
+        <v>41047505.3225</v>
       </c>
       <c r="O21">
-        <v>22819104.77894737</v>
+        <v>41216398.4475</v>
       </c>
       <c r="P21">
-        <v>4.536842105263158</v>
+        <v>1.3075</v>
       </c>
       <c r="Q21">
-        <v>2.284210526315789</v>
+        <v>1.26</v>
       </c>
       <c r="R21">
-        <v>29319616.44210526</v>
+        <v>26371341.6375</v>
       </c>
       <c r="S21">
-        <v>363462592.0210527</v>
+        <v>335689344.2125</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -1672,58 +1678,58 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>6238612.8</v>
+        <v>9459597.135</v>
       </c>
       <c r="C22">
-        <v>7207.094736842106</v>
+        <v>8982.51</v>
       </c>
       <c r="D22">
-        <v>120081929.4315789</v>
+        <v>118076243.5325</v>
       </c>
       <c r="E22">
-        <v>165925455.8736842</v>
+        <v>248577275.4975</v>
       </c>
       <c r="F22">
-        <v>83339.31578947368</v>
+        <v>129302.1375</v>
       </c>
       <c r="G22">
-        <v>1156160.421052632</v>
+        <v>831385.375</v>
       </c>
       <c r="H22">
-        <v>790013.8315789474</v>
+        <v>1255066.915</v>
       </c>
       <c r="I22">
-        <v>6125622.136842106</v>
+        <v>9653971.3675</v>
       </c>
       <c r="J22">
-        <v>2645730.736842105</v>
+        <v>4630882.1525</v>
       </c>
       <c r="K22">
-        <v>3557286.084210526</v>
+        <v>5340493.2375</v>
       </c>
       <c r="L22">
-        <v>247642.3789473684</v>
+        <v>94213.435</v>
       </c>
       <c r="M22">
-        <v>15480.03157894737</v>
+        <v>23198.2925</v>
       </c>
       <c r="N22">
-        <v>29189257.58947368</v>
+        <v>41479319.9125</v>
       </c>
       <c r="O22">
-        <v>33314445.90526316</v>
+        <v>41658272.8725</v>
       </c>
       <c r="P22">
-        <v>1.263157894736842</v>
+        <v>0.7875</v>
       </c>
       <c r="Q22">
-        <v>0.4315789473684211</v>
+        <v>0.7425</v>
       </c>
       <c r="R22">
-        <v>28640253.12631579</v>
+        <v>26799306.04</v>
       </c>
       <c r="S22">
-        <v>346234731.1894737</v>
+        <v>336426336.845</v>
       </c>
     </row>
     <row r="23" spans="1:19">
@@ -1731,58 +1737,58 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>4887825.095744681</v>
+        <v>7281162.583541147</v>
       </c>
       <c r="C23">
-        <v>8165.872340425532</v>
+        <v>11105.44139650873</v>
       </c>
       <c r="D23">
-        <v>115839355.2659574</v>
+        <v>118072455.6907731</v>
       </c>
       <c r="E23">
-        <v>175394353.712766</v>
+        <v>269146760.2518703</v>
       </c>
       <c r="F23">
-        <v>33558.29787234042</v>
+        <v>54303.34912718205</v>
       </c>
       <c r="G23">
-        <v>245526.9787234043</v>
+        <v>116929.3266832918</v>
       </c>
       <c r="H23">
-        <v>628117.0638297872</v>
+        <v>1064679.14713217</v>
       </c>
       <c r="I23">
-        <v>4693376.20212766</v>
+        <v>7092918.04488778</v>
       </c>
       <c r="J23">
-        <v>2655329.329787234</v>
+        <v>3980233.583541147</v>
       </c>
       <c r="K23">
-        <v>2799500.138297872</v>
+        <v>4060321.431421447</v>
       </c>
       <c r="L23">
-        <v>95100.56382978724</v>
+        <v>11165.23690773067</v>
       </c>
       <c r="M23">
-        <v>18588.89361702128</v>
+        <v>19319.3042394015</v>
       </c>
       <c r="N23">
-        <v>24596280.07446808</v>
+        <v>37441021.43890274</v>
       </c>
       <c r="O23">
-        <v>26156001.69148936</v>
+        <v>37598669.97506234</v>
       </c>
       <c r="P23">
-        <v>7.617021276595745</v>
+        <v>1.144638403990025</v>
       </c>
       <c r="Q23">
-        <v>2.265957446808511</v>
+        <v>1.167082294264339</v>
       </c>
       <c r="R23">
-        <v>22681118.36170213</v>
+        <v>27727808.14214464</v>
       </c>
       <c r="S23">
-        <v>351253479.4893617</v>
+        <v>342692197.5012469</v>
       </c>
     </row>
     <row r="24" spans="1:19">
@@ -1790,58 +1796,58 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>6359686.884210526</v>
+        <v>7256389.9125</v>
       </c>
       <c r="C24">
-        <v>11506.92631578947</v>
+        <v>11979.8</v>
       </c>
       <c r="D24">
-        <v>119101737.1894737</v>
+        <v>118033307.3875</v>
       </c>
       <c r="E24">
-        <v>228938490.4526316</v>
+        <v>270932145.2775</v>
       </c>
       <c r="F24">
-        <v>87995.51578947369</v>
+        <v>92231.8125</v>
       </c>
       <c r="G24">
-        <v>881554.1789473684</v>
+        <v>559265.3575</v>
       </c>
       <c r="H24">
-        <v>2850.2</v>
+        <v>2485.96</v>
       </c>
       <c r="I24">
-        <v>7215340.768421053</v>
+        <v>8551367.9725</v>
       </c>
       <c r="J24">
-        <v>4002068.726315789</v>
+        <v>5049169.27</v>
       </c>
       <c r="K24">
-        <v>4817233.452631579</v>
+        <v>5521662.575</v>
       </c>
       <c r="L24">
-        <v>187133.5368421053</v>
+        <v>58347.505</v>
       </c>
       <c r="M24">
-        <v>23569.64210526316</v>
+        <v>25244.2175</v>
       </c>
       <c r="N24">
-        <v>32319832.86315789</v>
+        <v>37332700.995</v>
       </c>
       <c r="O24">
-        <v>31183757.12631579</v>
+        <v>37492129.02</v>
       </c>
       <c r="P24">
-        <v>3.168421052631579</v>
+        <v>0.0675</v>
       </c>
       <c r="Q24">
-        <v>0.5684210526315789</v>
+        <v>0</v>
       </c>
       <c r="R24">
-        <v>28744168.77894737</v>
+        <v>28276586.72</v>
       </c>
       <c r="S24">
-        <v>346190477.3368421</v>
+        <v>345170340.635</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -1849,58 +1855,58 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>5768339.372340426</v>
+        <v>7225995.34</v>
       </c>
       <c r="C25">
-        <v>6811.765957446809</v>
+        <v>8540.4275</v>
       </c>
       <c r="D25">
-        <v>120176257.3617021</v>
+        <v>118125114.985</v>
       </c>
       <c r="E25">
-        <v>213244946.2234043</v>
+        <v>268962076.7375</v>
       </c>
       <c r="F25">
-        <v>71242.03191489361</v>
+        <v>91714.58749999999</v>
       </c>
       <c r="G25">
-        <v>756834.8617021276</v>
+        <v>704021.605</v>
       </c>
       <c r="H25">
-        <v>717673.1382978724</v>
+        <v>905080.465</v>
       </c>
       <c r="I25">
-        <v>6657231.212765957</v>
+        <v>8448662.744999999</v>
       </c>
       <c r="J25">
-        <v>3760828.127659575</v>
+        <v>4867517.4225</v>
       </c>
       <c r="K25">
-        <v>4435038.627659574</v>
+        <v>5432604.37</v>
       </c>
       <c r="L25">
-        <v>131803.9787234043</v>
+        <v>109986.765</v>
       </c>
       <c r="M25">
-        <v>22183.96808510638</v>
+        <v>24207.765</v>
       </c>
       <c r="N25">
-        <v>29961565.45744681</v>
+        <v>37723309.8175</v>
       </c>
       <c r="O25">
-        <v>37474989.25531915</v>
+        <v>37880663.4675</v>
       </c>
       <c r="P25">
-        <v>4.031914893617022</v>
+        <v>1.0125</v>
       </c>
       <c r="Q25">
-        <v>0.5425531914893617</v>
+        <v>0.6525</v>
       </c>
       <c r="R25">
-        <v>26972270.42553192</v>
+        <v>28639895.42</v>
       </c>
       <c r="S25">
-        <v>364340203.393617</v>
+        <v>342433846.3125</v>
       </c>
     </row>
     <row r="26" spans="1:19">
@@ -1908,58 +1914,58 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>9078659.126315789</v>
+        <v>9706524.5875</v>
       </c>
       <c r="C26">
-        <v>10839.24210526316</v>
+        <v>10823.78</v>
       </c>
       <c r="D26">
-        <v>117213598.8</v>
+        <v>118090900.7775</v>
       </c>
       <c r="E26">
-        <v>233816085.0631579</v>
+        <v>263027161.6525</v>
       </c>
       <c r="F26">
-        <v>17834.53684210526</v>
+        <v>12785.09</v>
       </c>
       <c r="G26">
-        <v>212569.9052631579</v>
+        <v>112722.0375</v>
       </c>
       <c r="H26">
-        <v>1261575.578947368</v>
+        <v>1523669.4425</v>
       </c>
       <c r="I26">
-        <v>7518608.368421053</v>
+        <v>8460145.805</v>
       </c>
       <c r="J26">
-        <v>3834831.042105263</v>
+        <v>4328124.0225</v>
       </c>
       <c r="K26">
-        <v>3946225.736842105</v>
+        <v>4393626.56</v>
       </c>
       <c r="L26">
-        <v>85044.85263157895</v>
+        <v>20435.7625</v>
       </c>
       <c r="M26">
-        <v>16690.52631578947</v>
+        <v>18372.6475</v>
       </c>
       <c r="N26">
-        <v>36240851.37894737</v>
+        <v>40678762.505</v>
       </c>
       <c r="O26">
-        <v>44464006.30526315</v>
+        <v>40854083.77</v>
       </c>
       <c r="P26">
-        <v>0.5894736842105263</v>
+        <v>0</v>
       </c>
       <c r="Q26">
-        <v>6.178947368421053</v>
+        <v>0.0225</v>
       </c>
       <c r="R26">
-        <v>23587331.25263158</v>
+        <v>24249467.88</v>
       </c>
       <c r="S26">
-        <v>358666588.0947368</v>
+        <v>349119230.755</v>
       </c>
     </row>
     <row r="27" spans="1:19">
@@ -1967,58 +1973,58 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>5466431.431578947</v>
+        <v>8905409.689999999</v>
       </c>
       <c r="C27">
-        <v>7827.547368421053</v>
+        <v>7952.39</v>
       </c>
       <c r="D27">
-        <v>120578320.2947368</v>
+        <v>118096560.6225</v>
       </c>
       <c r="E27">
-        <v>151281307.7157895</v>
+        <v>245897992.715</v>
       </c>
       <c r="F27">
-        <v>66511.83157894737</v>
+        <v>101261.235</v>
       </c>
       <c r="G27">
-        <v>1072430.568421053</v>
+        <v>933962.6775</v>
       </c>
       <c r="H27">
-        <v>2326.757894736842</v>
+        <v>2490.17</v>
       </c>
       <c r="I27">
-        <v>5379849.52631579</v>
+        <v>9919829.705</v>
       </c>
       <c r="J27">
-        <v>2901924.2</v>
+        <v>5473858.1825</v>
       </c>
       <c r="K27">
-        <v>3766271.484210526</v>
+        <v>6184272.79</v>
       </c>
       <c r="L27">
-        <v>236957.5052631579</v>
+        <v>188627.37</v>
       </c>
       <c r="M27">
-        <v>19265.62105263158</v>
+        <v>21823.36</v>
       </c>
       <c r="N27">
-        <v>22563087.8</v>
+        <v>37304393.0025</v>
       </c>
       <c r="O27">
-        <v>21149947.83157895</v>
+        <v>37460946.5225</v>
       </c>
       <c r="P27">
-        <v>17.45263157894737</v>
+        <v>0.9475</v>
       </c>
       <c r="Q27">
-        <v>0.1684210526315789</v>
+        <v>0.855</v>
       </c>
       <c r="R27">
-        <v>28556949.96842105</v>
+        <v>31534499.92</v>
       </c>
       <c r="S27">
-        <v>358738401.0210527</v>
+        <v>326601946.1225</v>
       </c>
     </row>
     <row r="28" spans="1:19">
@@ -2026,58 +2032,58 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>8781669.915789474</v>
+        <v>8957777.7875</v>
       </c>
       <c r="C28">
-        <v>11022.12631578947</v>
+        <v>10598.935</v>
       </c>
       <c r="D28">
-        <v>117688537.7473684</v>
+        <v>118096630.625</v>
       </c>
       <c r="E28">
-        <v>238840328.7684211</v>
+        <v>244931130.12</v>
       </c>
       <c r="F28">
-        <v>127320.8210526316</v>
+        <v>128565.8175</v>
       </c>
       <c r="G28">
-        <v>975343.2421052632</v>
+        <v>943630.795</v>
       </c>
       <c r="H28">
-        <v>1106792.768421053</v>
+        <v>1128812.305</v>
       </c>
       <c r="I28">
-        <v>9710689.105263159</v>
+        <v>9906585.602499999</v>
       </c>
       <c r="J28">
-        <v>5310384.705263158</v>
+        <v>5368786.6725</v>
       </c>
       <c r="K28">
-        <v>6366254.789473685</v>
+        <v>6157861.13</v>
       </c>
       <c r="L28">
-        <v>146764.2842105263</v>
+        <v>125949.4875</v>
       </c>
       <c r="M28">
-        <v>19188.96842105263</v>
+        <v>23520.03</v>
       </c>
       <c r="N28">
-        <v>38249666.83157895</v>
+        <v>38244774.9025</v>
       </c>
       <c r="O28">
-        <v>41653357.49473684</v>
+        <v>38406935.48</v>
       </c>
       <c r="P28">
-        <v>0.5052631578947369</v>
+        <v>1.35</v>
       </c>
       <c r="Q28">
-        <v>0.1894736842105263</v>
+        <v>0.9</v>
       </c>
       <c r="R28">
-        <v>31690531.63157895</v>
+        <v>31883532.3525</v>
       </c>
       <c r="S28">
-        <v>328014967.4631579</v>
+        <v>326787535.6875</v>
       </c>
     </row>
     <row r="29" spans="1:19">
@@ -2085,58 +2091,58 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>9775503.222222222</v>
+        <v>13876595.14285714</v>
       </c>
       <c r="C29">
-        <v>16590.77777777778</v>
+        <v>23047</v>
       </c>
       <c r="D29">
-        <v>117150321.6666667</v>
+        <v>116770672.8571429</v>
       </c>
       <c r="E29">
-        <v>188250221.6666667</v>
+        <v>241281764.4285714</v>
       </c>
       <c r="F29">
-        <v>208708.6666666667</v>
+        <v>311303.4285714286</v>
       </c>
       <c r="G29">
-        <v>336970.8888888889</v>
+        <v>442965.8571428572</v>
       </c>
       <c r="H29">
-        <v>1225340.444444444</v>
+        <v>1562794.428571429</v>
       </c>
       <c r="I29">
-        <v>1822632.888888889</v>
+        <v>1670958.714285714</v>
       </c>
       <c r="J29">
-        <v>1337611</v>
+        <v>1100310.142857143</v>
       </c>
       <c r="K29">
-        <v>1726219.555555556</v>
+        <v>1382791.857142857</v>
       </c>
       <c r="L29">
-        <v>97259.55555555556</v>
+        <v>84179.28571428571</v>
       </c>
       <c r="M29">
-        <v>15419.33333333333</v>
+        <v>14452.71428571429</v>
       </c>
       <c r="N29">
-        <v>11636304.33333333</v>
+        <v>15758444.85714286</v>
       </c>
       <c r="O29">
-        <v>12689828.44444444</v>
+        <v>16610324.42857143</v>
       </c>
       <c r="P29">
+        <v>14.42857142857143</v>
+      </c>
+      <c r="Q29">
         <v>0</v>
       </c>
-      <c r="Q29">
-        <v>68.77777777777777</v>
-      </c>
       <c r="R29">
-        <v>32567983</v>
+        <v>40539600.85714286</v>
       </c>
       <c r="S29">
-        <v>350496954.2222222</v>
+        <v>332332877.1428571</v>
       </c>
     </row>
     <row r="30" spans="1:19">
@@ -2144,58 +2150,58 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>5524689.826086956</v>
+        <v>8650699</v>
       </c>
       <c r="C30">
-        <v>5884.304347826087</v>
+        <v>6634.538461538462</v>
       </c>
       <c r="D30">
-        <v>125446141.9565217</v>
+        <v>117265651.5384615</v>
       </c>
       <c r="E30">
-        <v>131402658.826087</v>
+        <v>208486663.8461539</v>
       </c>
       <c r="F30">
-        <v>47891.86956521739</v>
+        <v>41776.53846153846</v>
       </c>
       <c r="G30">
-        <v>114563.2608695652</v>
+        <v>88055.84615384616</v>
       </c>
       <c r="H30">
-        <v>2863.086956521739</v>
+        <v>2596.923076923077</v>
       </c>
       <c r="I30">
-        <v>186471.1304347826</v>
+        <v>289276.2307692308</v>
       </c>
       <c r="J30">
-        <v>8293.130434782608</v>
+        <v>16962.84615384615</v>
       </c>
       <c r="K30">
-        <v>22550.5652173913</v>
+        <v>19531.46153846154</v>
       </c>
       <c r="L30">
-        <v>97485.95652173914</v>
+        <v>141749.0769230769</v>
       </c>
       <c r="M30">
-        <v>11828.91304347826</v>
+        <v>3284.769230769231</v>
       </c>
       <c r="N30">
-        <v>6931100.304347826</v>
+        <v>12449700.92307692</v>
       </c>
       <c r="O30">
-        <v>6864755.130434782</v>
+        <v>12853381</v>
       </c>
       <c r="P30">
-        <v>37.91304347826087</v>
+        <v>2.076923076923077</v>
       </c>
       <c r="Q30">
-        <v>16.39130434782609</v>
+        <v>0</v>
       </c>
       <c r="R30">
-        <v>34217600.17391305</v>
+        <v>49693884.76923077</v>
       </c>
       <c r="S30">
-        <v>350513459.5652174</v>
+        <v>293744132.7692308</v>
       </c>
     </row>
     <row r="31" spans="1:19">
@@ -2203,46 +2209,46 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>6585379</v>
+        <v>12475495</v>
       </c>
       <c r="C31">
-        <v>47937</v>
+        <v>52059</v>
       </c>
       <c r="D31">
-        <v>107038432</v>
+        <v>117377184</v>
       </c>
       <c r="E31">
-        <v>118540141</v>
+        <v>204739960</v>
       </c>
       <c r="F31">
-        <v>17244</v>
+        <v>6655</v>
       </c>
       <c r="G31">
-        <v>111282</v>
+        <v>91388</v>
       </c>
       <c r="H31">
-        <v>2865</v>
+        <v>2637</v>
       </c>
       <c r="I31">
-        <v>316104</v>
+        <v>497553</v>
       </c>
       <c r="J31">
-        <v>285609</v>
+        <v>453419</v>
       </c>
       <c r="K31">
-        <v>338765</v>
+        <v>535213</v>
       </c>
       <c r="L31">
-        <v>3539</v>
+        <v>2182</v>
       </c>
       <c r="M31">
-        <v>16803</v>
+        <v>17938</v>
       </c>
       <c r="N31">
-        <v>7726090</v>
+        <v>13236936</v>
       </c>
       <c r="O31">
-        <v>7753047</v>
+        <v>13310098</v>
       </c>
       <c r="P31">
         <v>0</v>
@@ -2251,10 +2257,10 @@
         <v>0</v>
       </c>
       <c r="R31">
-        <v>27153103</v>
+        <v>45949573</v>
       </c>
       <c r="S31">
-        <v>290749118</v>
+        <v>286937400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>